<commit_message>
added id to notable_events data
</commit_message>
<xml_diff>
--- a/data/PH_notable.xlsx
+++ b/data/PH_notable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\ph_climate_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A11A5C6-AE1D-4060-85C4-BE685591527C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75B5300-26F5-4C29-991E-C202CA7547AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="513" xr2:uid="{00110006-848D-494C-A072-69C7A4FA1923}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="notable_extreme_events" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">notable_extreme_events!$A$1:$P$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">notable_extreme_events!$B$1:$Q$77</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="197">
   <si>
     <t>Deaths</t>
   </si>
@@ -629,6 +629,9 @@
   </si>
   <si>
     <t>2004 QUEZON PROVINCE LANDSLIDES</t>
+  </si>
+  <si>
+    <t>event_id</t>
   </si>
 </sst>
 </file>
@@ -1018,1518 +1021,1745 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15F33B8-28A5-415A-8F29-F76F81F316F6}">
-  <dimension ref="A1:P77"/>
+  <dimension ref="A1:Q77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D65" sqref="D65"/>
+      <selection pane="bottomRight" activeCell="A77" sqref="A2:A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="20.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="124.140625" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="28.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="124.140625" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
         <v>18968</v>
       </c>
-      <c r="B2" s="4">
+      <c r="C2" s="4">
         <v>18973</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>991</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
         <v>19284</v>
       </c>
-      <c r="B3" s="4">
+      <c r="C3" s="4">
         <v>19290</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>995</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>19725</v>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
       </c>
       <c r="B4" s="4">
         <v>19725</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>44</v>
+      <c r="C4" s="4">
+        <v>19725</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>21551</v>
+    <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
       </c>
       <c r="B5" s="4">
         <v>21551</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>44</v>
+      <c r="C5" s="4">
+        <v>21551</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>58</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>21551</v>
+    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>21551</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>44</v>
+      <c r="C6" s="4">
+        <v>21551</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
         <v>23377</v>
       </c>
-      <c r="B7" s="4">
+      <c r="C7" s="4">
         <v>23742</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+    <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
         <v>24838</v>
       </c>
-      <c r="B8" s="4">
+      <c r="C8" s="4">
         <v>25204</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
         <v>25569</v>
       </c>
-      <c r="B9" s="4">
+      <c r="C9" s="4">
         <v>26298</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+    <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
         <v>26299</v>
       </c>
-      <c r="B10" s="4">
+      <c r="C10" s="4">
         <v>26665</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="Q10" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+    <row r="11" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
         <v>26481</v>
       </c>
-      <c r="B11" s="4">
+      <c r="C11" s="4">
         <v>26510</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="Q11" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
         <v>26665</v>
       </c>
-      <c r="B12" s="4">
+      <c r="C12" s="4">
         <v>27759</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
         <v>29346</v>
       </c>
-      <c r="B13" s="4">
+      <c r="C13" s="4">
         <v>29363</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="Q13" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+    <row r="14" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4">
         <v>29587</v>
       </c>
-      <c r="B14" s="4">
+      <c r="C14" s="4">
         <v>29617</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1">
         <v>200</v>
       </c>
-      <c r="N14" s="1">
+      <c r="O14" s="1">
         <v>140000</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="Q14" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+    <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
         <v>29905</v>
       </c>
-      <c r="B15" s="4">
+      <c r="C15" s="4">
         <v>29917.75</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="Q15" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="90" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+    <row r="16" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4">
         <v>29952</v>
       </c>
-      <c r="B16" s="4">
+      <c r="C16" s="4">
         <v>30317</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="Q16" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+    <row r="17" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
         <v>30180</v>
       </c>
-      <c r="B17" s="4">
+      <c r="C17" s="4">
         <v>30198</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="P17" s="2" t="s">
+      <c r="Q17" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+    <row r="18" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4">
         <v>30920</v>
       </c>
-      <c r="B18" s="4">
+      <c r="C18" s="4">
         <v>30931.75</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="P18" s="2" t="s">
+      <c r="Q18" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+    <row r="19" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
         <v>31637</v>
       </c>
-      <c r="B19" s="4">
+      <c r="C19" s="4">
         <v>31657</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="P19" s="3" t="s">
+      <c r="Q19" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+    <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4">
         <v>31640</v>
       </c>
-      <c r="B20" s="4">
+      <c r="C20" s="4">
         <v>31661.75</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="P20" s="2" t="s">
+      <c r="Q20" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4">
         <v>31964.5</v>
       </c>
-      <c r="B21" s="4">
+      <c r="C21" s="4">
         <v>31976</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="P21" s="2" t="s">
+      <c r="Q21" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4">
         <v>32097</v>
       </c>
-      <c r="B22" s="4">
+      <c r="C22" s="4">
         <v>32111.25</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="P22" s="2" t="s">
+      <c r="Q22" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4">
         <v>32120</v>
       </c>
-      <c r="B23" s="4">
+      <c r="C23" s="4">
         <v>32131.5</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="P23" s="2" t="s">
+      <c r="Q23" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+    <row r="24" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4">
         <v>32509</v>
       </c>
-      <c r="B24" s="4">
+      <c r="C24" s="4">
         <v>32874</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P24" s="2" t="s">
+      <c r="Q24" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+    <row r="25" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4">
         <v>33183</v>
       </c>
-      <c r="B25" s="4">
+      <c r="C25" s="4">
         <v>33195.5</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="P25" s="2" t="s">
+      <c r="Q25" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+    <row r="26" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4">
         <v>33451</v>
       </c>
-      <c r="B26" s="4">
+      <c r="C26" s="4">
         <v>33817</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P26" s="2" t="s">
+      <c r="Q26" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+    <row r="27" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4">
         <v>33495</v>
       </c>
-      <c r="B27" s="4">
+      <c r="C27" s="4">
         <v>33514.25</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="P27" s="2" t="s">
+      <c r="Q27" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+    <row r="28" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4">
         <v>33527</v>
       </c>
-      <c r="B28" s="4">
+      <c r="C28" s="4">
         <v>33545</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="P28" s="2" t="s">
+      <c r="Q28" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+    <row r="29" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4">
         <v>33542</v>
       </c>
-      <c r="B29" s="4">
+      <c r="C29" s="4">
         <v>33550.5</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="P29" s="2" t="s">
+      <c r="Q29" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+    <row r="30" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4">
         <v>34678.75</v>
       </c>
-      <c r="B30" s="4">
+      <c r="C30" s="4">
         <v>34695.25</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="P30" s="2" t="s">
+      <c r="Q30" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+    <row r="31" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4">
         <v>34948</v>
       </c>
-      <c r="B31" s="4">
+      <c r="C31" s="4">
         <v>29951</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="M31" s="1">
+      <c r="N31" s="1">
         <v>48</v>
       </c>
-      <c r="P31" s="2" t="s">
+      <c r="Q31" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+    <row r="32" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="4">
         <v>34992.25</v>
       </c>
-      <c r="B32" s="4">
+      <c r="C32" s="4">
         <v>35010.5</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="P32" s="2" t="s">
+      <c r="Q32" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+    <row r="33" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="4">
         <v>35551</v>
       </c>
-      <c r="B33" s="4">
+      <c r="C33" s="4">
         <v>35947</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="P33" s="2" t="s">
+      <c r="Q33" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+    <row r="34" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="4">
         <v>35977</v>
       </c>
-      <c r="B34" s="4">
+      <c r="C34" s="4">
         <v>36557</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P34" s="2" t="s">
+      <c r="Q34" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="4">
         <v>36075.75</v>
       </c>
-      <c r="B35" s="4">
+      <c r="C35" s="4">
         <v>36088</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="P35" s="2" t="s">
+      <c r="Q35" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+    <row r="36" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="4">
         <v>36079.75</v>
       </c>
-      <c r="B36" s="4">
+      <c r="C36" s="4">
         <v>36098</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="P36" s="2" t="s">
+      <c r="Q36" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>36374</v>
+    <row r="37" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>36</v>
       </c>
       <c r="B37" s="4">
         <v>36374</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="4">
+        <v>36374</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M37" s="1">
+      <c r="N37" s="1">
         <v>60</v>
       </c>
-      <c r="P37" s="2" t="s">
+      <c r="Q37" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4">
         <v>36526</v>
       </c>
-      <c r="B38" s="4">
+      <c r="C38" s="4">
         <v>37256</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+    <row r="39" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4">
         <v>37072</v>
       </c>
-      <c r="B39" s="4">
+      <c r="C39" s="4">
         <v>37079.75</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="P39" s="2" t="s">
+      <c r="Q39" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+    <row r="40" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4">
         <v>37765.25</v>
       </c>
-      <c r="B40" s="4">
+      <c r="C40" s="4">
         <v>37776.25</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D40" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="P40" s="2" t="s">
+      <c r="Q40" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+    <row r="41" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4">
         <v>38305</v>
       </c>
-      <c r="B41" s="4">
+      <c r="C41" s="4">
         <v>38324</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="M41" s="1">
+      <c r="N41" s="1">
         <v>176</v>
       </c>
-      <c r="N41" s="1">
+      <c r="O41" s="1">
         <v>11</v>
       </c>
-      <c r="O41" s="1">
+      <c r="P41" s="1">
         <v>53</v>
       </c>
-      <c r="P41" s="2" t="s">
+      <c r="Q41" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="90" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
-        <v>38765</v>
+    <row r="42" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>41</v>
       </c>
       <c r="B42" s="4">
         <v>38765</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="4">
+        <v>38765</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G42" s="1">
+      <c r="H42" s="1">
         <v>10.3375</v>
       </c>
-      <c r="H42" s="1">
+      <c r="I42" s="1">
         <v>125.0975</v>
       </c>
-      <c r="M42" s="1">
+      <c r="N42" s="1">
         <v>1000</v>
       </c>
-      <c r="N42" s="1">
+      <c r="O42" s="1">
         <v>28</v>
       </c>
-      <c r="P42" s="2" t="s">
+      <c r="Q42" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+    <row r="43" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="4">
         <v>39045.5</v>
       </c>
-      <c r="B43" s="4">
+      <c r="C43" s="4">
         <v>39057.125</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="P43" s="2" t="s">
+      <c r="Q43" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+    <row r="44" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="4">
         <v>39616.25</v>
       </c>
-      <c r="B44" s="4">
+      <c r="C44" s="4">
         <v>39626</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="P44" s="2" t="s">
+      <c r="Q44" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+    <row r="45" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="4">
         <v>40081</v>
       </c>
-      <c r="B45" s="4">
+      <c r="C45" s="4">
         <v>40086.75</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="P45" s="2" t="s">
+      <c r="Q45" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+    <row r="46" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="4">
         <v>40083</v>
       </c>
-      <c r="B46" s="4">
+      <c r="C46" s="4">
         <v>40100.75</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="P46" s="2" t="s">
+      <c r="Q46" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+    <row r="47" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="4">
         <v>40330</v>
       </c>
-      <c r="B47" s="4">
+      <c r="C47" s="4">
         <v>41030</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="K47" s="1">
+      <c r="L47" s="1">
         <v>900000000</v>
       </c>
-      <c r="M47" s="1">
+      <c r="N47" s="1">
         <v>42</v>
       </c>
-      <c r="N47" s="1">
+      <c r="O47" s="1">
         <v>8</v>
       </c>
-      <c r="O47" s="1">
+      <c r="P47" s="1">
         <v>5</v>
       </c>
-      <c r="P47" s="2" t="s">
+      <c r="Q47" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+    <row r="48" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="4">
         <v>40462.5</v>
       </c>
-      <c r="B48" s="4">
+      <c r="C48" s="4">
         <v>40475.25</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D48" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="P48" s="2" t="s">
+      <c r="Q48" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
+    <row r="49" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="4">
         <v>40809</v>
       </c>
-      <c r="B49" s="4">
+      <c r="C49" s="4">
         <v>40816.75</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D49" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="P49" s="2" t="s">
+      <c r="Q49" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+    <row r="50" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="4">
         <v>40878</v>
       </c>
-      <c r="B50" s="4">
+      <c r="C50" s="4">
         <v>40908</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L50" s="1">
+      <c r="M50" s="1">
         <v>80000</v>
       </c>
-      <c r="M50" s="1">
+      <c r="N50" s="1">
         <v>3</v>
       </c>
-      <c r="O50" s="1">
+      <c r="P50" s="1">
         <v>7</v>
       </c>
-      <c r="P50" s="2" t="s">
+      <c r="Q50" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+    <row r="51" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="4">
         <v>40888.75</v>
       </c>
-      <c r="B51" s="4">
+      <c r="C51" s="4">
         <v>40896.5</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D51" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="P51" s="2" t="s">
+      <c r="Q51" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="5">
+    <row r="52" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="5">
         <v>41127</v>
       </c>
-      <c r="B52" s="5">
+      <c r="C52" s="5">
         <v>41133</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>13</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>14</v>
       </c>
-      <c r="E52"/>
       <c r="F52"/>
       <c r="G52"/>
       <c r="H52"/>
-      <c r="I52">
+      <c r="I52"/>
+      <c r="J52">
         <v>1007.4</v>
       </c>
-      <c r="J52" t="s">
+      <c r="K52" t="s">
         <v>23</v>
       </c>
-      <c r="K52"/>
       <c r="L52"/>
-      <c r="P52" s="2" t="s">
+      <c r="M52"/>
+      <c r="Q52" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+    <row r="53" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="4">
         <v>41238.5</v>
       </c>
-      <c r="B53" s="4">
+      <c r="C53" s="4">
         <v>41252.25</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="P53" s="2" t="s">
+      <c r="Q53" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+    <row r="54" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="4">
         <v>41261</v>
       </c>
-      <c r="B54" s="4">
+      <c r="C54" s="4">
         <v>41266</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L54" s="1">
+      <c r="M54" s="1">
         <v>4792</v>
       </c>
-      <c r="M54" s="1">
+      <c r="N54" s="1">
         <v>4</v>
       </c>
-      <c r="N54" s="1">
+      <c r="O54" s="1">
         <v>9</v>
       </c>
-      <c r="P54" s="2" t="s">
+      <c r="Q54" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="4">
         <v>41503</v>
       </c>
-      <c r="B55" s="4">
+      <c r="C55" s="4">
         <v>41507</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>13</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I55" s="1">
+      <c r="J55" s="1">
         <v>1120.2</v>
       </c>
-      <c r="J55" s="1" t="s">
+      <c r="K55" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P55" s="2" t="s">
+      <c r="Q55" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+    <row r="56" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="4">
         <v>41523</v>
       </c>
-      <c r="B56" s="4">
+      <c r="C56" s="4">
         <v>41639</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="P56" s="2" t="s">
+      <c r="Q56" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
+    <row r="57" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="4">
         <v>41580.25</v>
       </c>
-      <c r="B57" s="4">
+      <c r="C57" s="4">
         <v>41589.5</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D57" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="P57" s="2" t="s">
+      <c r="Q57" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+    <row r="58" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="4">
         <v>41829.25</v>
       </c>
-      <c r="B58" s="4">
+      <c r="C58" s="4">
         <v>41840.25</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D58" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="P58" s="2" t="s">
+      <c r="Q58" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
+    <row r="59" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="4">
         <v>42278</v>
       </c>
-      <c r="B59" s="4">
+      <c r="C59" s="4">
         <v>42491</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="P59" s="2" t="s">
+      <c r="Q59" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
+    <row r="60" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" s="4">
         <v>42289</v>
       </c>
-      <c r="B60" s="4">
+      <c r="C60" s="4">
         <v>42298.25</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D60" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="P60" s="2" t="s">
+      <c r="Q60" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" s="4">
         <v>42621.75</v>
       </c>
-      <c r="B61" s="4">
+      <c r="C61" s="4">
         <v>42630.5</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D61" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="F61" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="P61" s="2" t="s">
+      <c r="Q61" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
+    <row r="62" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" s="4">
         <v>42657.25</v>
       </c>
-      <c r="B62" s="4">
+      <c r="C62" s="4">
         <v>42669.25</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D62" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="F62" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="P62" s="2" t="s">
+      <c r="Q62" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
+    <row r="63" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" s="4">
         <v>42724</v>
       </c>
-      <c r="B63" s="4">
+      <c r="C63" s="4">
         <v>42732.5</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D63" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="F63" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="P63" s="2" t="s">
+      <c r="Q63" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A64" s="4">
+    <row r="64" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" s="4">
         <v>43070</v>
       </c>
-      <c r="B64" s="4">
+      <c r="C64" s="4">
         <v>43100</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="E64" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L64" s="1">
+      <c r="M64" s="1">
         <v>70000</v>
       </c>
-      <c r="P64" s="2" t="s">
+      <c r="Q64" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
+    <row r="65" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" s="4">
         <v>43296</v>
       </c>
-      <c r="B65" s="4">
+      <c r="C65" s="4">
         <v>43304</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>13</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I65" s="1">
+      <c r="J65" s="1">
         <v>1097.4000000000001</v>
       </c>
-      <c r="J65" s="1" t="s">
+      <c r="K65" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P65" s="2" t="s">
+      <c r="Q65" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="B66" s="1">
+    <row r="66" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="C66" s="1">
         <v>1962</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D66" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="P66" s="2" t="s">
+      <c r="Q66" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="B67" s="1">
+    <row r="67" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="C67" s="1">
         <v>1966</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D67" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="P67" s="2" t="s">
+      <c r="Q67" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B68" s="1">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+      <c r="C68" s="1">
         <v>1967</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D68" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E68" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B69" s="1">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="C69" s="1">
         <v>1968</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D69" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P69" s="2" t="s">
+      <c r="Q69" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B70" s="1">
+    <row r="70" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="C70" s="1">
         <v>1970</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D70" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="P70" s="2" t="s">
+      <c r="Q70" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B71" s="1">
+    <row r="71" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="C71" s="1">
         <v>1970</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D71" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P71" s="2" t="s">
+      <c r="Q71" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B72" s="1">
+    <row r="72" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="C72" s="1">
         <v>1970</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D72" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E72" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P72" s="2" t="s">
+      <c r="Q72" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B73" s="1">
+    <row r="73" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="C73" s="1">
         <v>1974</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D73" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E73" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P73" s="2" t="s">
+      <c r="Q73" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B74" s="1">
+    <row r="74" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="C74" s="1">
         <v>1974</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D74" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E74" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="P74" s="2" t="s">
+      <c r="Q74" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B75" s="1">
+    <row r="75" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="C75" s="1">
         <v>1975</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D75" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E75" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="P75" s="2" t="s">
+      <c r="Q75" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B76" s="1">
+    <row r="76" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="C76" s="1">
         <v>1976</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D76" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E76" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P76" s="2" t="s">
+      <c r="Q76" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B77" s="1">
+    <row r="77" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="C77" s="1">
         <v>1978</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D77" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="P77" s="2" t="s">
+      <c r="Q77" s="2" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P77" xr:uid="{F15F33B8-28A5-415A-8F29-F76F81F316F6}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P77">
-      <sortCondition ref="A1:A77"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new media and added new locations per notable event & more
</commit_message>
<xml_diff>
--- a/data/PH_notable.xlsx
+++ b/data/PH_notable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\ph_climate_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75B5300-26F5-4C29-991E-C202CA7547AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C37B6C2-D6A3-4B27-9940-64017C9B9203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="513" xr2:uid="{00110006-848D-494C-A072-69C7A4FA1923}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="notable_extreme_events" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">notable_extreme_events!$B$1:$Q$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">notable_extreme_events!$A$1:$Q$77</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="199">
   <si>
     <t>Deaths</t>
   </si>
@@ -632,6 +632,12 @@
   </si>
   <si>
     <t>event_id</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>YOLANDA</t>
   </si>
 </sst>
 </file>
@@ -676,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -687,6 +693,7 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1024,10 +1031,10 @@
   <dimension ref="A1:Q77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="J46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A77" sqref="A2:A77"/>
+      <selection pane="bottomRight" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,7 +1049,7 @@
     <col min="8" max="9" width="20.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -1120,6 +1127,9 @@
       <c r="E2" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="N2" s="1">
         <v>991</v>
       </c>
@@ -1143,6 +1153,9 @@
       <c r="E3" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="N3" s="1">
         <v>995</v>
       </c>
@@ -1166,6 +1179,9 @@
       <c r="E4" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q4" s="2" t="s">
         <v>52</v>
       </c>
@@ -1186,6 +1202,9 @@
       <c r="E5" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="N5" s="1">
         <v>58</v>
       </c>
@@ -1209,6 +1228,9 @@
       <c r="E6" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q6" s="2" t="s">
         <v>54</v>
       </c>
@@ -1229,6 +1251,9 @@
       <c r="E7" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -1246,6 +1271,9 @@
       <c r="E8" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1266,6 +1294,9 @@
       <c r="E9" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1280,6 +1311,9 @@
       <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q10" s="2" t="s">
         <v>3</v>
       </c>
@@ -1300,6 +1334,9 @@
       <c r="E11" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="F11" s="1">
+        <v>10</v>
+      </c>
       <c r="Q11" s="2" t="s">
         <v>109</v>
       </c>
@@ -1320,6 +1357,9 @@
       <c r="E12" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="F12" s="1" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1360,6 +1400,9 @@
       <c r="E14" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="F14" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="N14" s="1">
         <v>200</v>
       </c>
@@ -1409,6 +1452,9 @@
       <c r="E16" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="F16" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q16" s="2" t="s">
         <v>4</v>
       </c>
@@ -1587,6 +1633,9 @@
       <c r="D24" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F24" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q24" s="2" t="s">
         <v>6</v>
       </c>
@@ -1627,6 +1676,9 @@
       <c r="D26" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F26" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q26" s="2" t="s">
         <v>7</v>
       </c>
@@ -1696,6 +1748,9 @@
       <c r="F29" s="1" t="s">
         <v>160</v>
       </c>
+      <c r="N29" s="1">
+        <v>5101</v>
+      </c>
       <c r="Q29" s="2" t="s">
         <v>87</v>
       </c>
@@ -1739,6 +1794,9 @@
       <c r="E31" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="F31" s="1">
+        <v>30</v>
+      </c>
       <c r="N31" s="1">
         <v>48</v>
       </c>
@@ -1785,6 +1843,9 @@
       <c r="E33" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="F33" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q33" s="2" t="s">
         <v>8</v>
       </c>
@@ -1802,6 +1863,9 @@
       <c r="D34" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F34" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q34" s="2" t="s">
         <v>10</v>
       </c>
@@ -1868,6 +1932,9 @@
       <c r="E37" s="1" t="s">
         <v>194</v>
       </c>
+      <c r="F37" s="1">
+        <v>36</v>
+      </c>
       <c r="N37" s="1">
         <v>60</v>
       </c>
@@ -1891,6 +1958,9 @@
       <c r="E38" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="F38" s="1" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="39" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
@@ -1954,6 +2024,12 @@
       <c r="E41" s="1" t="s">
         <v>195</v>
       </c>
+      <c r="F41" s="1">
+        <v>40</v>
+      </c>
+      <c r="L41" s="1">
+        <v>207500000</v>
+      </c>
       <c r="N41" s="1">
         <v>176</v>
       </c>
@@ -1983,6 +2059,9 @@
       <c r="E42" s="1" t="s">
         <v>120</v>
       </c>
+      <c r="F42" s="1">
+        <v>41</v>
+      </c>
       <c r="H42" s="1">
         <v>10.3375</v>
       </c>
@@ -2107,6 +2186,9 @@
       <c r="E47" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="F47" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="L47" s="1">
         <v>900000000</v>
       </c>
@@ -2185,6 +2267,9 @@
       <c r="E50" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="F50" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="M50" s="1">
         <v>80000</v>
       </c>
@@ -2217,6 +2302,9 @@
       <c r="F51" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="N51" s="1">
+        <v>1268</v>
+      </c>
       <c r="Q51" s="2" t="s">
         <v>100</v>
       </c>
@@ -2237,7 +2325,9 @@
       <c r="E52" t="s">
         <v>14</v>
       </c>
-      <c r="F52"/>
+      <c r="F52" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="G52"/>
       <c r="H52"/>
       <c r="I52"/>
@@ -2272,6 +2362,12 @@
       <c r="F53" s="1" t="s">
         <v>180</v>
       </c>
+      <c r="L53" s="6">
+        <v>43164250000</v>
+      </c>
+      <c r="N53" s="1">
+        <v>1248</v>
+      </c>
       <c r="Q53" s="2" t="s">
         <v>101</v>
       </c>
@@ -2292,6 +2388,9 @@
       <c r="E54" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="F54" s="1">
+        <v>53</v>
+      </c>
       <c r="M54" s="1">
         <v>4792</v>
       </c>
@@ -2321,6 +2420,9 @@
       <c r="E55" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="F55" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="J55" s="1">
         <v>1120.2</v>
       </c>
@@ -2347,6 +2449,9 @@
       <c r="E56" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="F56" s="1">
+        <v>55</v>
+      </c>
       <c r="Q56" s="2" t="s">
         <v>112</v>
       </c>
@@ -2370,6 +2475,15 @@
       <c r="F57" s="1" t="s">
         <v>181</v>
       </c>
+      <c r="G57" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="L57" s="1">
+        <v>95483130000</v>
+      </c>
+      <c r="N57" s="1">
+        <v>6300</v>
+      </c>
       <c r="Q57" s="2" t="s">
         <v>102</v>
       </c>
@@ -2413,6 +2527,9 @@
       <c r="E59" s="1" t="s">
         <v>187</v>
       </c>
+      <c r="F59" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q59" s="2" t="s">
         <v>9</v>
       </c>
@@ -2525,6 +2642,9 @@
       <c r="E64" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="F64" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="M64" s="1">
         <v>70000</v>
       </c>
@@ -2548,6 +2668,9 @@
       <c r="E65" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="F65" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="J65" s="1">
         <v>1097.4000000000001</v>
       </c>
@@ -2571,6 +2694,9 @@
       <c r="E66" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="F66" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q66" s="2" t="s">
         <v>57</v>
       </c>
@@ -2588,6 +2714,9 @@
       <c r="E67" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="F67" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q67" s="2" t="s">
         <v>58</v>
       </c>
@@ -2605,6 +2734,9 @@
       <c r="E68" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="F68" s="1" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
@@ -2619,6 +2751,9 @@
       <c r="E69" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="F69" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q69" s="2" t="s">
         <v>59</v>
       </c>
@@ -2636,6 +2771,9 @@
       <c r="E70" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="F70" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q70" s="2" t="s">
         <v>60</v>
       </c>
@@ -2653,6 +2791,9 @@
       <c r="E71" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="F71" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q71" s="2" t="s">
         <v>60</v>
       </c>
@@ -2670,6 +2811,9 @@
       <c r="E72" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="F72" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q72" s="2" t="s">
         <v>60</v>
       </c>
@@ -2687,6 +2831,9 @@
       <c r="E73" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F73" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q73" s="2" t="s">
         <v>75</v>
       </c>
@@ -2704,6 +2851,9 @@
       <c r="E74" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F74" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q74" s="2" t="s">
         <v>146</v>
       </c>
@@ -2721,6 +2871,9 @@
       <c r="E75" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="F75" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q75" s="2" t="s">
         <v>76</v>
       </c>
@@ -2738,6 +2891,9 @@
       <c r="E76" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="F76" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q76" s="2" t="s">
         <v>77</v>
       </c>
@@ -2755,11 +2911,15 @@
       <c r="E77" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="F77" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="Q77" s="2" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q77" xr:uid="{F15F33B8-28A5-415A-8F29-F76F81F316F6}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>